<commit_message>
Added descriptions and tags_0 column for featured items to rights vocabulary
</commit_message>
<xml_diff>
--- a/nr_vocabularies/fixtures/rights.xlsx
+++ b/nr_vocabularies/fixtures/rights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\taxonomie\nr-vocabularies\nr_vocabularies\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\NUŠL\SW\INVENIO 3\metadatové modely\nr-github\nr-vocabularies\nr_vocabularies\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2ACBB2-BCD5-4DD4-8CCA-9929E8BA243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3C1F8E-6151-4EB9-836A-C24136B9322F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="215">
   <si>
     <t>code</t>
   </si>
@@ -603,16 +603,135 @@
   <si>
     <t>Rights/Licenses</t>
   </si>
+  <si>
+    <t>props.acronym</t>
+  </si>
+  <si>
+    <t>description_cs</t>
+  </si>
+  <si>
+    <t>description_en</t>
+  </si>
+  <si>
+    <t>tags_0</t>
+  </si>
+  <si>
+    <t>featured</t>
+  </si>
+  <si>
+    <t>Toto je starší verze licencí (1.0). Pokud licencujete své vlastní dílo, které ještě nebylo pod žádnou licencí zveřejněno, doporučujeme místo toho použít některou z variant licence 4.0.</t>
+  </si>
+  <si>
+    <t>This is an older version of the license (1.0). If you are licensing your own work that has not yet been published under any license, we recommend using one of the 4.0 license variants instead.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora. V češtině: Uveďte autora; v angličtině Attribution; zkratka CC BY.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format, so long as attribution is given to the creator. The license allows for commercial use. Abbreviation CC BY.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozšiřovat odvozená díla pouze za podmínek identické či slučitelné licence, je nutné uvést autora. V češtině: Uveďte autora-Zachovejte licenci; v angličtině: Attribution-ShareAlike; zkratka CC BY-SA.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format, so long as attribution is given to the creator. The license allows for commercial use. If you remix, adapt, or build upon the material, you must license the modified material under identical terms. Abbreviation CC BY-SA.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora a pouze pro nevýdělečné účely. V češtině: Uveďte autora-Neužívejte komerčně; v angličtině: Attribution-NonCommercial; zkratka CC BY-NC.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format for noncommercial purposes only, and only so long as attribution is given to the creator. Abbreviation CC BY-NC.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo (případně z něj odvozená díla) pouze pro nevýdělečné účely a pouze za podmínek identické či slučitelné licence. Je nutné uvést autora. V češtině: Uveďte autora-Neužívejte dílo komerčně-Zachovejte licenci; v angličtině: Attribution-NonCommercial-ShareAlike; zkratka CC BY-NC-SA.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format for noncommercial purposes only, and only so long as attribution is given to the creator. If you remix, adapt, or build upon the material, you must license the modified material under identical terms. Abbreviation CC BY-NC-SA.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat pouze dílo v původní podobě, nikoli díla z něj odvozená, je nutné uvést autora. V češtině: Uveďte autora-Nezasahujte do díla; v angličtině: Attribution-NoDerivs; zkratka CC BY-ND.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to copy and distribute the material in any medium or format in unadapted form only, and only so long as attribution is given to the creator. The license allows for commercial use. Abbreviation CC BY-ND.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat pouze dílo v původní podobě, nikoli díla z něj odvozená, pouze pro nevýdělečné účely, je nutné uvést autora. V češtině: Uveďte autora-Neužívejte komerčně-Nezasahujte do díla; v angličtině: Attribution-Noncommercial-NoDerivs; zkratka CC BY-NC-ND.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to copy and distribute the material in any medium or format in unadapted form only, for noncommercial purposes only, and only so long as attribution is given to the creator. Abbreviation CC BY-NC-ND.</t>
+  </si>
+  <si>
+    <t>Toto je starší verze licencí 2.0. Pokud licencujete své vlastní dílo, které ještě nebylo pod žádnou licencí zveřejněno, doporučujeme místo toho použít některou z variant licence 4.0.</t>
+  </si>
+  <si>
+    <t>This is an older version of the license (2.0). If you are licensing your own work that has not yet been published under any license, we recommend using one of the 4.0 license variants instead.</t>
+  </si>
+  <si>
+    <t>Toto je starší verze licencí 2.5. Pokud licencujete své vlastní dílo, které ještě nebylo pod žádnou licencí zveřejněno, doporučujeme místo toho použít některou z variant licence 4.0.</t>
+  </si>
+  <si>
+    <t>This is an older version of the license (2.5). If you are licensing your own work that has not yet been published under any license, we recommend using one of the 4.0 license variants instead.</t>
+  </si>
+  <si>
+    <t>Toto je starší verze licencí 3.0, která byla adaptována pro český právní řád. Pokud licencujete své vlastní dílo, které ještě nebylo pod žádnou licencí zveřejněno, doporučujeme místo toho použít některou z variant licence 4.0.</t>
+  </si>
+  <si>
+    <t>This is an older version of the license (3.0). If you are licensing your own work that has not yet been published under any license, we recommend using one of the 4.0 license variants instead.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora. V češtině: Uveďte autora; v angličtině: Attribution; zkratka CC BY.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora a pouze pro nevýdělečné účely. V češtině: Uveďte autora-Neužívejte komerčně); v angličtině: Attribution-NonCommercial; zkratka CC BY-NC.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat pouze dílo v původní podobě, nikoli díla z něj odvozená, pouze pro nevýdělečné účely, je nutné uvést autora. V češtině: Uveďte autora-Neužívejte komerčně-Nezasahujte do díla; v angličtině: Attribution-NonCommercial-NoDerivs; zkratka CC BY-NC-ND.</t>
+  </si>
+  <si>
+    <t>Aktuální verze 4.0 existuje pouze jako mezinárodní, nebyla nutná adaptace do národních právních řádů.</t>
+  </si>
+  <si>
+    <t>The current version 4.0 exists only as an international version, no adaptation to national legal systems was necessary.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora. V češtině: Uveďte původ (v češtině dříve označováno jako Uveďte autora); v angličtině: Attribution; zkratka CC BY.</t>
+  </si>
+  <si>
+    <t>This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format, so long as attribution is given to the creator. The license allows for commercial use. Abbreviation CC BY</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozšiřovat odvozená díla pouze za podmínek identické či slučitelné licence, je nutné uvést autora. V češtině: Uveďte původ-Zachovejte licenci (v češtině dříve označováno jako Uveďte autora-Zachovejte licenci); v angličtině: Attribution-ShareAlike; zkratka CC BY-SA.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo a z něj odvozená díla pouze při uvedení autora a pouze pro nevýdělečné účely. V češtině: Uveďte původ-Neužívejte komerčně (v češtině dříve označováno jako Uveďte autora-Neužívejte komerčně); v angličtině: Attribution-NonCommercial; zkratka CC BY-NC.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat dílo (případně z něj odvozená díla) pouze pro nevýdělečné účely a pouze za podmínek identické či slučitelné licence. Je nutné uvést autora. V češtině: Uveďte původ-Neužívejte dílo komerčně-Zachovejte licenci (v češtině dříve označováno jako Uveďte autora-Neužívejte dílo komerčně-Zachovejte licenci); v angličtině: Attribution-NonCommercial-ShareAlike; zkratka CC BY-NC-SA.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat pouze dílo v původní podobě, nikoli díla z něj odvozená, je nutné uvést autora. V češtině: Uveďte původ-Nezpracovávejte (v češtině dříve označováno jako Uveďte autora-Nezasahujte do díla); v angličtině: Attribution-NoDerivs; zkratka BY-ND.</t>
+  </si>
+  <si>
+    <t>Umožňuje ostatním rozmnožovat, rozšiřovat, vystavovat a sdělovat pouze dílo v původní podobě, nikoli díla z něj odvozená, pouze pro nevýdělečné účely, je nutné uvést autora. V češtině: Uveďte původ-Neužívejte komerčně-Nezpracovávejte (v češtině dříve označováno jako Uveďte autora-Neužívejte komerčně-Nezasahujte do díla); v angličtině: Attribution-NonCommercial-NoDerivs; zkratka CC BY-NC-ND.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -624,6 +743,14 @@
       <sz val="11"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -709,26 +836,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální 2" xfId="1" xr:uid="{A544A385-974B-4915-821B-DCED555359E5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1888,27 +2019,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="86.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="72.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="52.21875" style="1" customWidth="1"/>
-    <col min="11" max="25" width="8.44140625" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.44140625" style="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="86.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="52.28515625" style="1" customWidth="1"/>
+    <col min="11" max="25" width="8.42578125" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15.6" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +2071,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="15.6" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>175</v>
       </c>
@@ -1972,7 +2103,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="13.5" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1998,7 +2129,7 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
     </row>
-    <row r="4" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="13.5" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -2024,7 +2155,7 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
     </row>
-    <row r="5" spans="1:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15.6" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -2043,10 +2174,18 @@
       <c r="F5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -2062,7 +2201,7 @@
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
     </row>
-    <row r="6" spans="1:24" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15.6" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2233,7 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
     </row>
-    <row r="7" spans="1:24" ht="15.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="15.4" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2109,9 +2248,15 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -2128,7 +2273,7 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
     </row>
-    <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -2147,9 +2292,15 @@
       <c r="F8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>186</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -2166,7 +2317,7 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="13.5" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2185,9 +2336,15 @@
       <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -2204,7 +2361,7 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
     </row>
-    <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="13.5" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -2223,9 +2380,15 @@
       <c r="F10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -2242,7 +2405,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -2261,9 +2424,15 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="J11" s="3"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -2280,7 +2449,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -2299,9 +2468,15 @@
       <c r="F12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -2318,7 +2493,7 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="13.5" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
@@ -2337,9 +2512,15 @@
       <c r="F13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2356,7 +2537,7 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="1:24" ht="15.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15.4" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
@@ -2371,9 +2552,15 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -2390,7 +2577,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>46</v>
       </c>
@@ -2409,9 +2596,15 @@
       <c r="F15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>186</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -2428,7 +2621,7 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="13.5" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>51</v>
       </c>
@@ -2447,9 +2640,15 @@
       <c r="F16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -2466,7 +2665,7 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="13.5" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -2485,9 +2684,15 @@
       <c r="F17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -2504,7 +2709,7 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="13.5" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>61</v>
       </c>
@@ -2523,9 +2728,15 @@
       <c r="F18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -2542,7 +2753,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>66</v>
       </c>
@@ -2561,9 +2772,15 @@
       <c r="F19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -2580,7 +2797,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="13.5" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
@@ -2599,9 +2816,15 @@
       <c r="F20" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -2618,7 +2841,7 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="1:24" ht="15.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="15.4" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>76</v>
       </c>
@@ -2633,9 +2856,15 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>200</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -2652,7 +2881,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="13.5" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>79</v>
       </c>
@@ -2671,9 +2900,15 @@
       <c r="F22" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>186</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -2690,7 +2925,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="13.5" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>84</v>
       </c>
@@ -2709,9 +2944,15 @@
       <c r="F23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -2728,7 +2969,7 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>89</v>
       </c>
@@ -2747,9 +2988,15 @@
       <c r="F24" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -2766,7 +3013,7 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
-    <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>94</v>
       </c>
@@ -2785,9 +3032,15 @@
       <c r="F25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -2804,7 +3057,7 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
     </row>
-    <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="13.5" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -2823,9 +3076,15 @@
       <c r="F26" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -2842,7 +3101,7 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
-    <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>104</v>
       </c>
@@ -2861,9 +3120,15 @@
       <c r="F27" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -2880,7 +3145,7 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:24" ht="15.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="15.4" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>109</v>
       </c>
@@ -2895,9 +3160,15 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>202</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -2914,7 +3185,7 @@
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
     </row>
-    <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="13.5" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>112</v>
       </c>
@@ -2933,9 +3204,15 @@
       <c r="F29" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>186</v>
+      </c>
       <c r="J29" s="3"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
@@ -2952,7 +3229,7 @@
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
     </row>
-    <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="13.5" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>117</v>
       </c>
@@ -2971,9 +3248,15 @@
       <c r="F30" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>188</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -2990,7 +3273,7 @@
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
     </row>
-    <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="13.5" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>122</v>
       </c>
@@ -3009,9 +3292,15 @@
       <c r="F31" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -3028,7 +3317,7 @@
       <c r="W31" s="6"/>
       <c r="X31" s="6"/>
     </row>
-    <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="13.5" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>127</v>
       </c>
@@ -3047,9 +3336,15 @@
       <c r="F32" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
@@ -3066,7 +3361,7 @@
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
     </row>
-    <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="13.5" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>132</v>
       </c>
@@ -3085,9 +3380,15 @@
       <c r="F33" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>194</v>
+      </c>
       <c r="J33" s="3"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -3104,7 +3405,7 @@
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
     </row>
-    <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>137</v>
       </c>
@@ -3123,9 +3424,15 @@
       <c r="F34" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="6"/>
+      <c r="G34" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>196</v>
+      </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -3142,7 +3449,7 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" spans="1:24" ht="15.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="15.4" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>142</v>
       </c>
@@ -3157,9 +3464,15 @@
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="6"/>
+      <c r="G35" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -3176,7 +3489,7 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
     </row>
-    <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="13.5" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>145</v>
       </c>
@@ -3195,10 +3508,18 @@
       <c r="F36" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="3"/>
+      <c r="G36" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -3214,7 +3535,7 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="13.5" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>150</v>
       </c>
@@ -3233,10 +3554,18 @@
       <c r="F37" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="3"/>
+      <c r="G37" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -3252,7 +3581,7 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="13.5" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>155</v>
       </c>
@@ -3271,10 +3600,18 @@
       <c r="F38" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="3"/>
+      <c r="G38" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -3290,7 +3627,7 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="13.5" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>160</v>
       </c>
@@ -3309,10 +3646,18 @@
       <c r="F39" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="3"/>
+      <c r="G39" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -3328,7 +3673,7 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
-    <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="13.5" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>165</v>
       </c>
@@ -3347,10 +3692,18 @@
       <c r="F40" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="3"/>
+      <c r="G40" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -3366,7 +3719,7 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="13.5" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>170</v>
       </c>
@@ -3385,10 +3738,18 @@
       <c r="F41" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="3"/>
+      <c r="G41" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -3404,7 +3765,7 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="13.5" customHeight="1">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="3"/>

</xml_diff>